<commit_message>
confirmed and updated referral and patiemt modules
</commit_message>
<xml_diff>
--- a/mapping/mml_patient_module_mapping.xlsx
+++ b/mapping/mml_patient_module_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="23475" windowHeight="9780"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="20730" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -289,10 +289,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>master id/checkDigitShema</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>other id/Identifier</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -472,10 +468,6 @@
     <t>MML0003</t>
   </si>
   <si>
-    <t>Telecom type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mmlPh:area</t>
   </si>
   <si>
@@ -500,10 +492,6 @@
     <t>mmlPh:extension</t>
   </si>
   <si>
-    <t>structured_telecoms/extention</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mmlPh:full</t>
   </si>
   <si>
@@ -537,15 +525,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Address type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>*nationality/primary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>*nationality/seconday</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -842,12 +822,32 @@
     <t>/items[openEHR-EHR-CLUSTER.individual_personal-mml.v1 and name/value='Individual's personal demographics for MML expression']/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0.20]/value</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>master id/checkDigitSchema</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*nationality/secondary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Address type with HL7 table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Telecoms type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>structured_telecoms/extension</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,8 +863,17 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,6 +883,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -907,7 +922,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -934,6 +949,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1296,10 +1323,10 @@
         <v>79</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -1358,10 +1385,10 @@
         <v>81</v>
       </c>
       <c r="J7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
@@ -1381,10 +1408,10 @@
         <v>82</v>
       </c>
       <c r="J8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
@@ -1401,10 +1428,10 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="J9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
@@ -1415,10 +1442,10 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="J10" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
@@ -1438,10 +1465,10 @@
         <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
@@ -1457,14 +1484,14 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="I12" t="s">
-        <v>84</v>
+      <c r="I12" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="J12" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
@@ -1497,13 +1524,13 @@
         <v>19</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
@@ -1520,13 +1547,13 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
@@ -1543,13 +1570,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="I16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K16" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -1560,10 +1587,10 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="J17" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1580,7 +1607,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="K18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1597,13 +1624,13 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="I19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K19" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1620,13 +1647,13 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
@@ -1656,7 +1683,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="H22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J22" s="8"/>
     </row>
@@ -1664,7 +1691,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
@@ -1673,23 +1700,23 @@
         <v>18</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="J23" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="K23" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
@@ -1700,13 +1727,13 @@
       <c r="F24" s="1"/>
       <c r="J24" s="8"/>
       <c r="K24" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
@@ -1715,19 +1742,19 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="I25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K25" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
@@ -1736,19 +1763,19 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="I26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K26" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
@@ -1759,19 +1786,19 @@
       </c>
       <c r="F27" s="1"/>
       <c r="I27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
@@ -1780,19 +1807,19 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="I28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
@@ -1803,19 +1830,19 @@
       </c>
       <c r="F29" s="1"/>
       <c r="I29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K29" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
@@ -1826,13 +1853,13 @@
       </c>
       <c r="F30" s="1"/>
       <c r="I30" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K30" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
@@ -1852,13 +1879,13 @@
         <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="K31" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
@@ -1877,13 +1904,13 @@
         <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K32" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
@@ -1902,13 +1929,13 @@
       </c>
       <c r="F33" s="1"/>
       <c r="I33" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K33" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.15">
@@ -1924,8 +1951,8 @@
         <v>36</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="I34" s="4" t="s">
-        <v>156</v>
+      <c r="I34" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="J34" s="8"/>
     </row>
@@ -1945,16 +1972,16 @@
       </c>
       <c r="F35" s="1"/>
       <c r="H35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K35" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.15">
@@ -1971,13 +1998,13 @@
       </c>
       <c r="F36" s="1"/>
       <c r="I36" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K36" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
@@ -1994,13 +2021,13 @@
       </c>
       <c r="F37" s="1"/>
       <c r="I37" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K37" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.15">
@@ -2024,13 +2051,13 @@
         <v>80</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K38" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.15">
@@ -2061,14 +2088,14 @@
       </c>
       <c r="F40" s="1"/>
       <c r="H40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>13</v>
@@ -2077,23 +2104,23 @@
         <v>18</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K41" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>13</v>
@@ -2102,23 +2129,23 @@
         <v>36</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K42" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>13</v>
@@ -2128,14 +2155,14 @@
       </c>
       <c r="F43" s="5"/>
       <c r="K43" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L43" s="7"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
@@ -2146,19 +2173,19 @@
       </c>
       <c r="F44" s="5"/>
       <c r="I44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K44" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
@@ -2169,19 +2196,19 @@
       </c>
       <c r="F45" s="5"/>
       <c r="I45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J45" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K45" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
@@ -2192,19 +2219,19 @@
       </c>
       <c r="F46" s="5"/>
       <c r="I46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J46" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K46" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5" t="s">
@@ -2215,19 +2242,19 @@
       </c>
       <c r="F47" s="5"/>
       <c r="I47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J47" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K47" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
@@ -2238,19 +2265,19 @@
       </c>
       <c r="F48" s="5"/>
       <c r="I48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J48" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K48" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
@@ -2261,19 +2288,19 @@
       </c>
       <c r="F49" s="5"/>
       <c r="I49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J49" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K49" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
@@ -2284,13 +2311,13 @@
       </c>
       <c r="F50" s="5"/>
       <c r="I50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J50" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K50" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.15">
@@ -2307,7 +2334,7 @@
       </c>
       <c r="F51" s="1"/>
       <c r="H51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.15">
@@ -2326,13 +2353,13 @@
       </c>
       <c r="F52" s="1"/>
       <c r="I52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J52" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K52" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.15">
@@ -2363,14 +2390,14 @@
       </c>
       <c r="F54" s="1"/>
       <c r="H54" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>13</v>
@@ -2379,22 +2406,22 @@
         <v>36</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>227</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="K55" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
@@ -2405,19 +2432,19 @@
       </c>
       <c r="F56" s="1"/>
       <c r="I56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J56" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K56" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
@@ -2428,19 +2455,19 @@
       </c>
       <c r="F57" s="1"/>
       <c r="I57" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K57" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
@@ -2451,19 +2478,19 @@
       </c>
       <c r="F58" s="1"/>
       <c r="I58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K58" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
@@ -2473,20 +2500,20 @@
         <v>34</v>
       </c>
       <c r="F59" s="1"/>
-      <c r="I59" t="s">
-        <v>144</v>
+      <c r="I59" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="J59" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K59" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
@@ -2497,19 +2524,19 @@
       </c>
       <c r="F60" s="1"/>
       <c r="I60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J60" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K60" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
@@ -2520,19 +2547,19 @@
       </c>
       <c r="F61" s="1"/>
       <c r="I61" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J61" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K61" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
@@ -2543,13 +2570,13 @@
       </c>
       <c r="F62" s="1"/>
       <c r="I62" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K62" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.15">
@@ -2571,13 +2598,13 @@
         <v>80</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K63" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.15">
@@ -2596,13 +2623,13 @@
       </c>
       <c r="F64" s="1"/>
       <c r="I64" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J64" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K64" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.15">
@@ -2621,16 +2648,16 @@
       </c>
       <c r="F65" s="1"/>
       <c r="H65" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K65" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="27" x14ac:dyDescent="0.15">
@@ -2647,18 +2674,19 @@
       </c>
       <c r="F66" s="1"/>
       <c r="I66" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="K66" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>